<commit_message>
changed inertial elements to calculated ones, fixed inertia of left_hip_yaw, temporarily added gazebo launch files for testing
</commit_message>
<xml_diff>
--- a/robotis_humanoid_description/doc/robotis_humanoid.xlsx
+++ b/robotis_humanoid_description/doc/robotis_humanoid.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="584" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="292" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="160201" sheetId="1" state="visible" r:id="rId2"/>
@@ -1026,23 +1026,25 @@
   </sheetPr>
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H48" activeCellId="0" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.6137339055794"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.412017167382"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.6137339055794"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.4077253218884"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="8.6137339055794"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.75107296137339"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.75107296137339"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.75107296137339"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8326180257511"/>
-    <col collapsed="false" hidden="false" max="20" min="18" style="0" width="10"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.6137339055794"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.61133603238866"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.412955465587"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.61133603238866"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.412955465587"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="8.61133603238866"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.75708502024292"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.75708502024292"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.75708502024292"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.834008097166"/>
+    <col collapsed="false" hidden="false" max="20" min="18" style="0" width="9.99595141700405"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.61133603238866"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3211,7 +3213,7 @@
         <v>0.24302997</v>
       </c>
       <c r="H48" s="105" t="n">
-        <v>0.012</v>
+        <v>-0.012</v>
       </c>
       <c r="I48" s="105" t="n">
         <v>0</v>
@@ -3663,7 +3665,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.6137339055794"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.61133603238866"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>